<commit_message>
AIP-2106 AIP-2110  Updated partial circuit files and code for the same
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/RMS_Data_Validation_Cablings/3U4U.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/RMS_Data_Validation_Cablings/3U4U.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4645AA5E-0227-46B5-A515-0CEE10CC03A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FD93D4-57D7-42ED-A622-52E1AF8240C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -269,9 +269,6 @@
     <t>sn409026540_7U_11I.cal</t>
   </si>
   <si>
-    <t>Cabling 3U4U</t>
-  </si>
-  <si>
     <t>Busbar_Channel_Map</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>DSP_2_Feeder_Map_2</t>
+  </si>
+  <si>
+    <t>Cabling 4U3U</t>
   </si>
 </sst>
 </file>
@@ -781,15 +781,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="2">
         <v>-1</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" s="2">
         <v>-1</v>
@@ -855,15 +855,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1">
         <v>4</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="1">
         <v>10</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1">
         <v>11</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="1">
         <v>12</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1">
         <v>6</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="1">
         <v>7</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20">
         <v>13</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24">
         <v>14</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25">
         <v>15</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26">
         <v>16</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30">
         <v>17</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31">
         <v>18</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1191,7 +1191,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1284,7 +1284,7 @@
         <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -1993,7 +1993,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>